<commit_message>
add 2 papers about scheduling
</commit_message>
<xml_diff>
--- a/软件定义建模与执行/content.xlsx
+++ b/软件定义建模与执行/content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\实验室相关\人机物\论文\RelatedWorks\软件定义建模与执行\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B715F6-50DA-4BDC-8F03-93600F0BE30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E479C3B7-30E0-4D91-8CBB-4B7D93496433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8820" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="223" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Reactive Microservices for the Internet of Things: A case study in Fog Computing</t>
   </si>
@@ -121,6 +121,37 @@
   </si>
   <si>
     <t>https://ieeexplore.ieee.org/abstract/document/8114554</t>
+  </si>
+  <si>
+    <t>Ming Yang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Multi-Objective Task Scheduling Method for Fog Computing in Cyber-Physical-Social Services</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fog computing provides users with data storage, computing, and other services by using fog layer devices close to edge devices. Tasks and resource scheduling in fog computing has become a research hotspot. For the multi-objective task-scheduling problem in fog computing, an adaptive multi-objective optimization task scheduling method for fog computing (FOG-AMOSM) is proposed in this paper. In this method, the total execution time and the task resource cost in the fog network are taken as the optimization target of resource allocation, and a multi-objective task scheduling model is designed. Since the objective model is a Pareto optimal solution problem, the global optimal solution can be obtained by using multi-objective optimization theory and the improved multi-objective evolutionary heuristic algorithm. Moreover, to obtain a better distribution of the current task scheduling group, the neighborhood is adaptively changed according to the current situation of the task scheduling group in fog computing, which avoids the problem that the neighborhood value caused by the neighborhood policy in the multi-objective algorithm affects the distribution of the task scheduling population. This algorithm is used to solve the non-inferior solution set of the utility function index of fog computing task scheduling to try to solve the multi-objective cooperative optimization problem in fog computing task scheduling. The results show that the proposed method has better performance than other methods in terms of total task execution time, resource cost and load dimensions.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9049337</t>
+  </si>
+  <si>
+    <t>A two-layer optimal scheduling framework for energy savings in a data center for Cyber–Physical–Social Systems</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QingxiaZhang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S138376212100045X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In recent years, big data and data analytics based on Cyber–Physical–Social Systems (CPSS) have become increasingly popular in providing valued services to humans. For many applications of CPSS, adequate computing infrastructure, which can be realized using powerful data centers (DCs), is needed. These DCs can then provide CPSS application developers with flexible and efficient High-Performance-Computing-Communications services. In DCs, the energy consumption of the cooling system which dissipates the heat generated by information technology (IT) devices should be optimized. Since the cooling system is one of the main energy consumers of DCs, optimization of its energy consumption can drastically reduce the operating costs while maintaining stable operation of the IT devices by efficient heat dissipation. Therefore, there is continuing development on improving the performance of cooling systems for DCs using different optimization strategies. In particular, model-based optimization algorithms have had impressive advances, but their deployment in real physical systems often becomes difficult due to limited data, poor optimization efficiency, and potential operation risks. In this paper, we propose a two-layer optimal scheduling framework for room-level cooling of DCs. In the global layer, we use limited data to build a set of novel physically-based empirical models to achieve accurate system energy tracking. Then with defined equipment operating constraints, a genetic algorithm efficiently obtains the optimal plan of all equipment control while ensuring safe system operations. In the local layer, through interactions with the global layer, local precision air conditioners are regulated to stabilize the room temperature within a safe range. To test our solution in a real physical system, we deployed the two-layer optimal scheduling technique in the real DC cooling system of Postal Savings Bank of China in Hefei, China. Our solution achieved an impressive average reduction of 6.1% on cooling load factor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -472,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -485,7 +516,7 @@
     <col min="3" max="3" width="18.53125" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.73046875" style="1" customWidth="1"/>
     <col min="5" max="5" width="180.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.53125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="59.06640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
@@ -609,12 +640,53 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B7" s="5"/>
+    <row r="7" spans="1:6" ht="97.15" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="124.9" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1" location="!" display="https://www.sciencedirect.com/science/article/pii/S138376212100045X - !" xr:uid="{63565379-90DB-4248-8221-A72BE6EDC9F3}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{4C1D034B-C713-4558-87FB-151FB0C6AC0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>